<commit_message>
Commit Assignment01 upload 1
</commit_message>
<xml_diff>
--- a/jupyter/Assignment01/2021-06-city-of-london-street.xlsx
+++ b/jupyter/Assignment01/2021-06-city-of-london-street.xlsx
@@ -3078,8 +3078,8 @@
   <sheetPr/>
   <dimension ref="A1:L571"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3088,7 +3088,11 @@
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="11.875" customWidth="1"/>
     <col min="4" max="4" width="9.875" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
     <col min="8" max="8" width="10.25" customWidth="1"/>
+    <col min="9" max="9" width="17.875" customWidth="1"/>
+    <col min="10" max="10" width="24.375" customWidth="1"/>
+    <col min="11" max="11" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">

</xml_diff>